<commit_message>
Combined all chart data into 2 charts, one log scale and one linear scale.
</commit_message>
<xml_diff>
--- a/chartsnstuff.xlsx
+++ b/chartsnstuff.xlsx
@@ -133,12 +133,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Random</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Data Sorting Time (linear scale)</a:t>
+              <a:t>Data Sorting Time (linear scale)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -194,7 +190,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>mergesortRandom</c:v>
+            <c:v>Mergesort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -208,11 +204,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="00B0F0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -398,7 +394,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>insertionSortRandom</c:v>
+            <c:v>Insertionsort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -602,7 +598,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>bubblesortRandom</c:v>
+            <c:v>Bubblesort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -802,6 +798,1230 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Mergesort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000119</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.000193</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000248</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000364</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.000553</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.00109</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.001609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Insertionsort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7E-6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Bubblesort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>0.000145</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>0.000284</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>0.000562</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.001115</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>0.00222</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>0.004456</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.008892</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.01769</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.035487</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.071541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Mergesort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$53:$A$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>7E-6</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00E+00">
+                  <c:v>1.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>2.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00E+00">
+                  <c:v>3.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00E+00">
+                  <c:v>4.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00E+00">
+                  <c:v>5.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00E+00">
+                  <c:v>8.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000247</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.000176</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000251</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000379</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.001129</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.000747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.001664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Insertionsort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$53:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>1.7E-5</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00E+00">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>7.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000165</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00E+00">
+                  <c:v>0.000324</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.000615</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.002434</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00E+00">
+                  <c:v>0.00412</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.004594</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.009153</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00E+00">
+                  <c:v>0.018534</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.040605</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.071939</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.00E+00">
+                  <c:v>0.144877</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.292046</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Bubblesort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$53:$C$78</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>0.000182</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>0.000366</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>0.000727</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>0.003067</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>0.003859</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.005548</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>0.010924</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>0.022608</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.045358</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.086206</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.17617</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.363274</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -810,11 +2030,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125180864"/>
-        <c:axId val="-2125173488"/>
+        <c:axId val="-2121262896"/>
+        <c:axId val="-2043048064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125180864"/>
+        <c:axId val="-2121262896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +2118,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -932,12 +2152,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125173488"/>
+        <c:crossAx val="-2043048064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125173488"/>
+        <c:axId val="-2043048064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +2270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125180864"/>
+        <c:crossAx val="-2121262896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1842,11 +3062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089076624"/>
-        <c:axId val="-2089585680"/>
+        <c:axId val="-2039987168"/>
+        <c:axId val="-2040061792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089076624"/>
+        <c:axId val="-2039987168"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1964,12 +3184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089585680"/>
+        <c:crossAx val="-2040061792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089585680"/>
+        <c:axId val="-2040061792"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2083,7 +3303,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089076624"/>
+        <c:crossAx val="-2039987168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2871,11 +4091,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111697920"/>
-        <c:axId val="-2064566880"/>
+        <c:axId val="-2114459440"/>
+        <c:axId val="-2114018672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111697920"/>
+        <c:axId val="-2114459440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2993,12 +4213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064566880"/>
+        <c:crossAx val="-2114018672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2064566880"/>
+        <c:axId val="-2114018672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,7 +4331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2111697920"/>
+        <c:crossAx val="-2114459440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3899,11 +5119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2044241232"/>
-        <c:axId val="-2044178368"/>
+        <c:axId val="-2043610576"/>
+        <c:axId val="-2043300032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2044241232"/>
+        <c:axId val="-2043610576"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4022,12 +5242,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044178368"/>
+        <c:crossAx val="-2043300032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2044178368"/>
+        <c:axId val="-2043300032"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4141,7 +5361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044241232"/>
+        <c:crossAx val="-2043610576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4929,11 +6149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079381168"/>
-        <c:axId val="-2079644832"/>
+        <c:axId val="-2043313728"/>
+        <c:axId val="-2121059088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079381168"/>
+        <c:axId val="-2043313728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5051,12 +6271,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079644832"/>
+        <c:crossAx val="-2121059088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2079644832"/>
+        <c:axId val="-2121059088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5169,7 +6389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079381168"/>
+        <c:crossAx val="-2043313728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5957,11 +7177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2065223920"/>
-        <c:axId val="-2079558576"/>
+        <c:axId val="-2112503968"/>
+        <c:axId val="-2129086784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2065223920"/>
+        <c:axId val="-2112503968"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6080,12 +7300,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079558576"/>
+        <c:crossAx val="-2129086784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2079558576"/>
+        <c:axId val="-2129086784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6199,7 +7419,2261 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065223920"/>
+        <c:crossAx val="-2112503968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Data Sorting Time (logarithmic scale)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.185714317141455"/>
+          <c:y val="0.115581384766399"/>
+          <c:w val="0.452313626812244"/>
+          <c:h val="0.755343634681349"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Mergesort Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000208</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.000109</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000156</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000181</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.000277</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000327</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000475</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.000708</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.001018</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.001438</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.002136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Insertionsort Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000145</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000285</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.000469</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.000731</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.001259</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.002363</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.004475</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.009017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.024576</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.037686</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.074845</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.15388</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Bubblesort Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.000117</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000236</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.000379</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.000791</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.001161</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.002339</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.004327</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.008884</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.019024</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.041476</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.079338</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.158942</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.321442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Mergesort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000119</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.000193</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000248</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000364</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.000553</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.000784</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.00109</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.001609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Insertionsort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7E-6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Bubblesort Presorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>0.000145</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>0.000284</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>0.000562</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.001115</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>0.00222</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>0.004456</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.008892</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.01769</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.035487</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.071541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Mergesort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$53:$A$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>6E-6</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>7E-6</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00E+00">
+                  <c:v>1.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>2.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00E+00">
+                  <c:v>3.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00E+00">
+                  <c:v>4.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00E+00">
+                  <c:v>5.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00E+00">
+                  <c:v>8.3E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.000247</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.000176</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.000251</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.000379</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.001129</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.000747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.00108</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.001664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Insertionsort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$53:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>9E-6</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00E+00">
+                  <c:v>1.7E-5</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00E+00">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00E+00">
+                  <c:v>7.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.000165</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00E+00">
+                  <c:v>0.000324</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.000615</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.002434</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00E+00">
+                  <c:v>0.00412</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.004594</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.009153</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00E+00">
+                  <c:v>0.018534</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.040605</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.071939</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.00E+00">
+                  <c:v>0.144877</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.292046</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Bubblesort Reverse Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$53:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1448.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2896.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5793.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$53:$C$78</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>0.000182</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>0.000366</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>0.000727</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>0.003067</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>0.003859</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>0.005548</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>0.010924</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>0.022608</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>0.045358</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.086206</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>0.17617</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>0.363274</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2040522544"/>
+        <c:axId val="-2045071664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2040522544"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>data</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size (4-byte integers)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2045071664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2045071664"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2040522544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6520,6 +9994,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9616,20 +13130,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
+      <xdr:colOff>184660</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>98381</xdr:rowOff>
+      <xdr:rowOff>66231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>17888</xdr:rowOff>
+      <xdr:colOff>489460</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>175434</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9650,16 +13680,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>609814</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>214702</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>149577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>158125</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>526062</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>59346</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9795,6 +13825,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>125393</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>119853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>430193</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>31500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10072,7 +14132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F50" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="150" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved comments and pseudocode.
</commit_message>
<xml_diff>
--- a/chartsnstuff.xlsx
+++ b/chartsnstuff.xlsx
@@ -2030,11 +2030,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121262896"/>
-        <c:axId val="-2043048064"/>
+        <c:axId val="-2071135552"/>
+        <c:axId val="-2096650064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2121262896"/>
+        <c:axId val="-2071135552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,12 +2152,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043048064"/>
+        <c:crossAx val="-2096650064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2043048064"/>
+        <c:axId val="-2096650064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2233,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2270,7 +2270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121262896"/>
+        <c:crossAx val="-2071135552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3062,11 +3062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2039987168"/>
-        <c:axId val="-2040061792"/>
+        <c:axId val="-2074572448"/>
+        <c:axId val="-2090677680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2039987168"/>
+        <c:axId val="-2074572448"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3184,12 +3184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2040061792"/>
+        <c:crossAx val="-2090677680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2040061792"/>
+        <c:axId val="-2090677680"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3303,7 +3303,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2039987168"/>
+        <c:crossAx val="-2074572448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4091,11 +4091,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114459440"/>
-        <c:axId val="-2114018672"/>
+        <c:axId val="-2077055840"/>
+        <c:axId val="-2068347936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2114459440"/>
+        <c:axId val="-2077055840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4213,12 +4213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114018672"/>
+        <c:crossAx val="-2068347936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2114018672"/>
+        <c:axId val="-2068347936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4331,7 +4331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114459440"/>
+        <c:crossAx val="-2077055840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5119,11 +5119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2043610576"/>
-        <c:axId val="-2043300032"/>
+        <c:axId val="-2071415584"/>
+        <c:axId val="-2067605264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2043610576"/>
+        <c:axId val="-2071415584"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5242,12 +5242,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043300032"/>
+        <c:crossAx val="-2067605264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2043300032"/>
+        <c:axId val="-2067605264"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5361,7 +5361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043610576"/>
+        <c:crossAx val="-2071415584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5483,7 +5483,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -6149,11 +6148,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2043313728"/>
-        <c:axId val="-2121059088"/>
+        <c:axId val="-2075248224"/>
+        <c:axId val="-2076296144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2043313728"/>
+        <c:axId val="-2075248224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6204,7 +6203,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6271,12 +6269,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121059088"/>
+        <c:crossAx val="-2076296144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2121059088"/>
+        <c:axId val="-2076296144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6322,7 +6320,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6389,7 +6386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2043313728"/>
+        <c:crossAx val="-2075248224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6403,7 +6400,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6511,7 +6507,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -7177,11 +7172,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112503968"/>
-        <c:axId val="-2129086784"/>
+        <c:axId val="-2090840496"/>
+        <c:axId val="-2116062944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112503968"/>
+        <c:axId val="-2090840496"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7233,7 +7228,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7300,12 +7294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129086784"/>
+        <c:crossAx val="-2116062944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2129086784"/>
+        <c:axId val="-2116062944"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -7352,7 +7346,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7419,7 +7412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112503968"/>
+        <c:crossAx val="-2090840496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7433,7 +7426,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9431,11 +9423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2040522544"/>
-        <c:axId val="-2045071664"/>
+        <c:axId val="-2071268848"/>
+        <c:axId val="-2114008272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2040522544"/>
+        <c:axId val="-2071268848"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -9554,12 +9546,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045071664"/>
+        <c:crossAx val="-2114008272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0"/>
+        <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2045071664"/>
+        <c:axId val="-2114008272"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -9636,7 +9630,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9673,8 +9667,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2040522544"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-2071268848"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -14132,7 +14126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Started the write up in write-up.docx.
</commit_message>
<xml_diff>
--- a/chartsnstuff.xlsx
+++ b/chartsnstuff.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\cs2500\cs2500project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TOSHIBA/cs2500/Assignments/Project 1/cs2500project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25680" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,14 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -182,8 +185,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.185714317141455"/>
           <c:y val="0.115581384766399"/>
-          <c:w val="0.45231362681224402"/>
-          <c:h val="0.75534363468134902"/>
+          <c:w val="0.452313626812244"/>
+          <c:h val="0.755343634681349"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -224,82 +227,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,82 +314,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>462</c:v>
+                  <c:v>462.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>499637</c:v>
+                  <c:v>499637.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12969</c:v>
+                  <c:v>12969.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14619</c:v>
+                  <c:v>14619.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17177</c:v>
+                  <c:v>17177.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21219</c:v>
+                  <c:v>21219.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25130</c:v>
+                  <c:v>25130.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33066</c:v>
+                  <c:v>33066.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47091</c:v>
+                  <c:v>47091.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55193</c:v>
+                  <c:v>55193.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120945</c:v>
+                  <c:v>120945.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119724</c:v>
+                  <c:v>119724.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>163334</c:v>
+                  <c:v>163334.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>208643</c:v>
+                  <c:v>208643.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>333745</c:v>
+                  <c:v>333745.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>458238</c:v>
+                  <c:v>458238.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>691812</c:v>
+                  <c:v>691812.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>970926</c:v>
+                  <c:v>970926.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1420930</c:v>
+                  <c:v>1.42093E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1344560</c:v>
+                  <c:v>1.34456E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2066550</c:v>
+                  <c:v>2.06655E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1070740</c:v>
+                  <c:v>1.07074E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1576650</c:v>
+                  <c:v>1.57665E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2230900</c:v>
+                  <c:v>2.2309E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3309100</c:v>
+                  <c:v>3.3091E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4714960</c:v>
+                  <c:v>4.71496E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -428,82 +431,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,82 +518,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>891</c:v>
+                  <c:v>891.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1369</c:v>
+                  <c:v>1369.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2145</c:v>
+                  <c:v>2145.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2887</c:v>
+                  <c:v>2887.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4505</c:v>
+                  <c:v>4505.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7260</c:v>
+                  <c:v>7260.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11154</c:v>
+                  <c:v>11154.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17787</c:v>
+                  <c:v>17787.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25773</c:v>
+                  <c:v>25773.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55786</c:v>
+                  <c:v>55786.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92186</c:v>
+                  <c:v>92186.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184536</c:v>
+                  <c:v>184536.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313681</c:v>
+                  <c:v>313681.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>659818</c:v>
+                  <c:v>659818.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1216860</c:v>
+                  <c:v>1.21686E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2475030</c:v>
+                  <c:v>2.47503E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5016480</c:v>
+                  <c:v>5.01648E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9859690</c:v>
+                  <c:v>9.85969E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12931900</c:v>
+                  <c:v>1.29319E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25145300</c:v>
+                  <c:v>2.51453E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26792000</c:v>
+                  <c:v>2.6792E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44076100</c:v>
+                  <c:v>4.40761E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>81560000</c:v>
+                  <c:v>8.156E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>160177000</c:v>
+                  <c:v>1.60177E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>279019000</c:v>
+                  <c:v>2.79019E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -632,82 +635,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -719,82 +722,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>775</c:v>
+                  <c:v>775.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039</c:v>
+                  <c:v>1039.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1667</c:v>
+                  <c:v>1667.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2392</c:v>
+                  <c:v>2392.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3861</c:v>
+                  <c:v>3861.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6055</c:v>
+                  <c:v>6055.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9586</c:v>
+                  <c:v>9586.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17803</c:v>
+                  <c:v>17803.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28165</c:v>
+                  <c:v>28165.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51051</c:v>
+                  <c:v>51051.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96063</c:v>
+                  <c:v>96063.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>161667</c:v>
+                  <c:v>161667.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>321123</c:v>
+                  <c:v>321123.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>585832</c:v>
+                  <c:v>585832.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1140530</c:v>
+                  <c:v>1.14053E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2137790</c:v>
+                  <c:v>2.13779E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4177390</c:v>
+                  <c:v>4.17739E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8186760</c:v>
+                  <c:v>8.18676E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13010900</c:v>
+                  <c:v>1.30109E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20966400</c:v>
+                  <c:v>2.09664E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27186200</c:v>
+                  <c:v>2.71862E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>55541100</c:v>
+                  <c:v>5.55411E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>70755200</c:v>
+                  <c:v>7.07552E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>149668000</c:v>
+                  <c:v>1.49668E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>266394000</c:v>
+                  <c:v>2.66394E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>555069000</c:v>
+                  <c:v>5.55069E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,82 +839,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,82 +926,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424</c:v>
+                  <c:v>424.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>872</c:v>
+                  <c:v>872.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>896</c:v>
+                  <c:v>896.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35034</c:v>
+                  <c:v>35034.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2012</c:v>
+                  <c:v>2012.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3024</c:v>
+                  <c:v>3024.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3700</c:v>
+                  <c:v>3700.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18348</c:v>
+                  <c:v>18348.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6736</c:v>
+                  <c:v>6736.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10916</c:v>
+                  <c:v>10916.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17036</c:v>
+                  <c:v>17036.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31204</c:v>
+                  <c:v>31204.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34656</c:v>
+                  <c:v>34656.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49300</c:v>
+                  <c:v>49300.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74376</c:v>
+                  <c:v>74376.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104764</c:v>
+                  <c:v>104764.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>147752</c:v>
+                  <c:v>147752.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>221676</c:v>
+                  <c:v>221676.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>312292</c:v>
+                  <c:v>312292.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>476340</c:v>
+                  <c:v>476340.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>673732</c:v>
+                  <c:v>673732.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1006000</c:v>
+                  <c:v>1.006E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1424090</c:v>
+                  <c:v>1.42409E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1905310</c:v>
+                  <c:v>1.90531E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2699150</c:v>
+                  <c:v>2.69915E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,82 +1043,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,82 +1130,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>308</c:v>
+                  <c:v>308.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156</c:v>
+                  <c:v>156.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>176</c:v>
+                  <c:v>176.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>196</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216</c:v>
+                  <c:v>216.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>284</c:v>
+                  <c:v>284.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>352</c:v>
+                  <c:v>352.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>428</c:v>
+                  <c:v>428.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>556</c:v>
+                  <c:v>556.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>720</c:v>
+                  <c:v>720.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>948</c:v>
+                  <c:v>948.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1296</c:v>
+                  <c:v>1296.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1708</c:v>
+                  <c:v>1708.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2380</c:v>
+                  <c:v>2380.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3328</c:v>
+                  <c:v>3328.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41262</c:v>
+                  <c:v>41262.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43047</c:v>
+                  <c:v>43047.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9176</c:v>
+                  <c:v>9176.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12928</c:v>
+                  <c:v>12928.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54357</c:v>
+                  <c:v>54357.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59876</c:v>
+                  <c:v>59876.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36336</c:v>
+                  <c:v>36336.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51352</c:v>
+                  <c:v>51352.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72816</c:v>
+                  <c:v>72816.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,82 +1247,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,82 +1334,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236</c:v>
+                  <c:v>236.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>392</c:v>
+                  <c:v>392.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>440</c:v>
+                  <c:v>440.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>552</c:v>
+                  <c:v>552.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>748</c:v>
+                  <c:v>748.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1048</c:v>
+                  <c:v>1048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1680</c:v>
+                  <c:v>1680.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2836</c:v>
+                  <c:v>2836.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4768</c:v>
+                  <c:v>4768.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45847</c:v>
+                  <c:v>45847.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58577</c:v>
+                  <c:v>58577.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107438</c:v>
+                  <c:v>107438.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>66480</c:v>
+                  <c:v>66480.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>204302</c:v>
+                  <c:v>204302.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>333571</c:v>
+                  <c:v>333571.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>512276</c:v>
+                  <c:v>512276.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1094920</c:v>
+                  <c:v>1.09492E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2102100</c:v>
+                  <c:v>2.1021E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4084700</c:v>
+                  <c:v>4.0847E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7777260</c:v>
+                  <c:v>7.77726E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26097200</c:v>
+                  <c:v>2.60972E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50709400</c:v>
+                  <c:v>5.07094E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76291900</c:v>
+                  <c:v>7.62919E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>137391000</c:v>
+                  <c:v>1.37391E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250417000</c:v>
+                  <c:v>2.50417E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,82 +1451,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1535,82 +1538,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>92</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>816</c:v>
+                  <c:v>816.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>684</c:v>
+                  <c:v>684.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>24776</c:v>
+                  <c:v>24776.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1452</c:v>
+                  <c:v>1452.0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1836</c:v>
+                  <c:v>1836.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2848</c:v>
+                  <c:v>2848.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3572</c:v>
+                  <c:v>3572.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>52305</c:v>
+                  <c:v>52305.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>29403</c:v>
+                  <c:v>29403.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>44484</c:v>
+                  <c:v>44484.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>71131</c:v>
+                  <c:v>71131.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>101508</c:v>
+                  <c:v>101508.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>142824</c:v>
+                  <c:v>142824.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>236131</c:v>
+                  <c:v>236131.0</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>293518</c:v>
+                  <c:v>293518.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>418489</c:v>
+                  <c:v>418489.0</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>607794</c:v>
+                  <c:v>607794.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>727373</c:v>
+                  <c:v>727373.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1302790</c:v>
+                  <c:v>1.30279E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>469364</c:v>
+                  <c:v>469364.0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1821350</c:v>
+                  <c:v>1.82135E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>980792</c:v>
+                  <c:v>980792.0</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1406840</c:v>
+                  <c:v>1.40684E6</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1857820</c:v>
+                  <c:v>1.85782E6</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>2650960</c:v>
+                  <c:v>2.65096E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,82 +1655,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,82 +1742,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>396</c:v>
+                  <c:v>396.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>576</c:v>
+                  <c:v>576.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1004</c:v>
+                  <c:v>1004.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1572</c:v>
+                  <c:v>1572.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2236</c:v>
+                  <c:v>2236.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3628</c:v>
+                  <c:v>3628.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>26829</c:v>
+                  <c:v>26829.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>45425</c:v>
+                  <c:v>45425.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>80883</c:v>
+                  <c:v>80883.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>158994</c:v>
+                  <c:v>158994.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>317724</c:v>
+                  <c:v>317724.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>622512</c:v>
+                  <c:v>622512.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1226590</c:v>
+                  <c:v>1.22659E6</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>2433140</c:v>
+                  <c:v>2.43314E6</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4877550</c:v>
+                  <c:v>4.87755E6</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>9721900</c:v>
+                  <c:v>9.7219E6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>17846500</c:v>
+                  <c:v>1.78465E7</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>24192500</c:v>
+                  <c:v>2.41925E7</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>27404700</c:v>
+                  <c:v>2.74047E7</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>57176400</c:v>
+                  <c:v>5.71764E7</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>76641300</c:v>
+                  <c:v>7.66413E7</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>143156000</c:v>
+                  <c:v>1.43156E8</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>286863000</c:v>
+                  <c:v>2.86863E8</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>559201000</c:v>
+                  <c:v>5.59201E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1856,82 +1859,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1943,82 +1946,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>192.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>336</c:v>
+                  <c:v>336.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>456</c:v>
+                  <c:v>456.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>592</c:v>
+                  <c:v>592.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>964</c:v>
+                  <c:v>964.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1408</c:v>
+                  <c:v>1408.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2444</c:v>
+                  <c:v>2444.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14966</c:v>
+                  <c:v>14966.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26169</c:v>
+                  <c:v>26169.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44500</c:v>
+                  <c:v>44500.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84595</c:v>
+                  <c:v>84595.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>167871</c:v>
+                  <c:v>167871.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>330231</c:v>
+                  <c:v>330231.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>647361</c:v>
+                  <c:v>647361.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1288800</c:v>
+                  <c:v>1.2888E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2570020</c:v>
+                  <c:v>2.57002E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5112610</c:v>
+                  <c:v>5.11261E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10049800</c:v>
+                  <c:v>1.00498E7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13852800</c:v>
+                  <c:v>1.38528E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9463410</c:v>
+                  <c:v>9.46341E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40634300</c:v>
+                  <c:v>4.06343E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48241400</c:v>
+                  <c:v>4.82414E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>85835600</c:v>
+                  <c:v>8.58356E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>169027000</c:v>
+                  <c:v>1.69027E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>302730000</c:v>
+                  <c:v>3.0273E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>571163000</c:v>
+                  <c:v>5.71163E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,11 +2036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="194738648"/>
-        <c:axId val="194739040"/>
+        <c:axId val="-2140950224"/>
+        <c:axId val="-2140958752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="194738648"/>
+        <c:axId val="-2140950224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,12 +2158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194739040"/>
+        <c:crossAx val="-2140958752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194739040"/>
+        <c:axId val="-2140958752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,7 +2276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194738648"/>
+        <c:crossAx val="-2140950224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2287,7 +2290,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.692030511284582"/>
+          <c:y val="0.338188296695473"/>
+          <c:w val="0.307969488715418"/>
+          <c:h val="0.451079837492784"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2434,8 +2446,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.185714317141455"/>
           <c:y val="0.115581384766399"/>
-          <c:w val="0.45231362681224402"/>
-          <c:h val="0.75534363468134902"/>
+          <c:w val="0.452313626812244"/>
+          <c:h val="0.755343634681349"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2476,82 +2488,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2563,82 +2575,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>462</c:v>
+                  <c:v>462.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>499637</c:v>
+                  <c:v>499637.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12969</c:v>
+                  <c:v>12969.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14619</c:v>
+                  <c:v>14619.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17177</c:v>
+                  <c:v>17177.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21219</c:v>
+                  <c:v>21219.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25130</c:v>
+                  <c:v>25130.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33066</c:v>
+                  <c:v>33066.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47091</c:v>
+                  <c:v>47091.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55193</c:v>
+                  <c:v>55193.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120945</c:v>
+                  <c:v>120945.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119724</c:v>
+                  <c:v>119724.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>163334</c:v>
+                  <c:v>163334.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>208643</c:v>
+                  <c:v>208643.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>333745</c:v>
+                  <c:v>333745.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>458238</c:v>
+                  <c:v>458238.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>691812</c:v>
+                  <c:v>691812.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>970926</c:v>
+                  <c:v>970926.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1420930</c:v>
+                  <c:v>1.42093E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1344560</c:v>
+                  <c:v>1.34456E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2066550</c:v>
+                  <c:v>2.06655E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1070740</c:v>
+                  <c:v>1.07074E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1576650</c:v>
+                  <c:v>1.57665E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2230900</c:v>
+                  <c:v>2.2309E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3309100</c:v>
+                  <c:v>3.3091E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4714960</c:v>
+                  <c:v>4.71496E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2680,82 +2692,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2767,82 +2779,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>891</c:v>
+                  <c:v>891.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1369</c:v>
+                  <c:v>1369.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2145</c:v>
+                  <c:v>2145.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2887</c:v>
+                  <c:v>2887.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4505</c:v>
+                  <c:v>4505.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7260</c:v>
+                  <c:v>7260.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11154</c:v>
+                  <c:v>11154.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17787</c:v>
+                  <c:v>17787.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25773</c:v>
+                  <c:v>25773.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55786</c:v>
+                  <c:v>55786.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92186</c:v>
+                  <c:v>92186.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184536</c:v>
+                  <c:v>184536.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313681</c:v>
+                  <c:v>313681.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>659818</c:v>
+                  <c:v>659818.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1216860</c:v>
+                  <c:v>1.21686E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2475030</c:v>
+                  <c:v>2.47503E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5016480</c:v>
+                  <c:v>5.01648E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9859690</c:v>
+                  <c:v>9.85969E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12931900</c:v>
+                  <c:v>1.29319E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25145300</c:v>
+                  <c:v>2.51453E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26792000</c:v>
+                  <c:v>2.6792E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44076100</c:v>
+                  <c:v>4.40761E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>81560000</c:v>
+                  <c:v>8.156E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>160177000</c:v>
+                  <c:v>1.60177E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>279019000</c:v>
+                  <c:v>2.79019E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2884,82 +2896,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2971,82 +2983,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>775</c:v>
+                  <c:v>775.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039</c:v>
+                  <c:v>1039.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1667</c:v>
+                  <c:v>1667.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2392</c:v>
+                  <c:v>2392.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3861</c:v>
+                  <c:v>3861.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6055</c:v>
+                  <c:v>6055.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9586</c:v>
+                  <c:v>9586.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17803</c:v>
+                  <c:v>17803.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28165</c:v>
+                  <c:v>28165.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51051</c:v>
+                  <c:v>51051.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96063</c:v>
+                  <c:v>96063.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>161667</c:v>
+                  <c:v>161667.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>321123</c:v>
+                  <c:v>321123.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>585832</c:v>
+                  <c:v>585832.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1140530</c:v>
+                  <c:v>1.14053E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2137790</c:v>
+                  <c:v>2.13779E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4177390</c:v>
+                  <c:v>4.17739E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8186760</c:v>
+                  <c:v>8.18676E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13010900</c:v>
+                  <c:v>1.30109E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20966400</c:v>
+                  <c:v>2.09664E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27186200</c:v>
+                  <c:v>2.71862E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>55541100</c:v>
+                  <c:v>5.55411E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>70755200</c:v>
+                  <c:v>7.07552E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>149668000</c:v>
+                  <c:v>1.49668E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>266394000</c:v>
+                  <c:v>2.66394E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>555069000</c:v>
+                  <c:v>5.55069E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3088,82 +3100,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3175,82 +3187,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424</c:v>
+                  <c:v>424.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>872</c:v>
+                  <c:v>872.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>896</c:v>
+                  <c:v>896.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35034</c:v>
+                  <c:v>35034.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2012</c:v>
+                  <c:v>2012.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3024</c:v>
+                  <c:v>3024.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3700</c:v>
+                  <c:v>3700.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18348</c:v>
+                  <c:v>18348.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6736</c:v>
+                  <c:v>6736.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10916</c:v>
+                  <c:v>10916.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17036</c:v>
+                  <c:v>17036.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31204</c:v>
+                  <c:v>31204.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34656</c:v>
+                  <c:v>34656.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49300</c:v>
+                  <c:v>49300.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74376</c:v>
+                  <c:v>74376.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104764</c:v>
+                  <c:v>104764.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>147752</c:v>
+                  <c:v>147752.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>221676</c:v>
+                  <c:v>221676.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>312292</c:v>
+                  <c:v>312292.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>476340</c:v>
+                  <c:v>476340.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>673732</c:v>
+                  <c:v>673732.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1006000</c:v>
+                  <c:v>1.006E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1424090</c:v>
+                  <c:v>1.42409E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1905310</c:v>
+                  <c:v>1.90531E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2699150</c:v>
+                  <c:v>2.69915E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3292,82 +3304,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3379,82 +3391,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>308</c:v>
+                  <c:v>308.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152</c:v>
+                  <c:v>152.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156</c:v>
+                  <c:v>156.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>176</c:v>
+                  <c:v>176.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>196</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216</c:v>
+                  <c:v>216.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>284</c:v>
+                  <c:v>284.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>352</c:v>
+                  <c:v>352.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>428</c:v>
+                  <c:v>428.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>556</c:v>
+                  <c:v>556.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>720</c:v>
+                  <c:v>720.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>948</c:v>
+                  <c:v>948.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1296</c:v>
+                  <c:v>1296.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1708</c:v>
+                  <c:v>1708.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2380</c:v>
+                  <c:v>2380.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3328</c:v>
+                  <c:v>3328.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41262</c:v>
+                  <c:v>41262.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43047</c:v>
+                  <c:v>43047.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9176</c:v>
+                  <c:v>9176.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12928</c:v>
+                  <c:v>12928.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54357</c:v>
+                  <c:v>54357.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59876</c:v>
+                  <c:v>59876.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36336</c:v>
+                  <c:v>36336.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51352</c:v>
+                  <c:v>51352.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72816</c:v>
+                  <c:v>72816.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3496,82 +3508,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3583,82 +3595,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236</c:v>
+                  <c:v>236.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>392</c:v>
+                  <c:v>392.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>440</c:v>
+                  <c:v>440.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>552</c:v>
+                  <c:v>552.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>748</c:v>
+                  <c:v>748.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1048</c:v>
+                  <c:v>1048.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1680</c:v>
+                  <c:v>1680.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2836</c:v>
+                  <c:v>2836.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4768</c:v>
+                  <c:v>4768.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45847</c:v>
+                  <c:v>45847.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58577</c:v>
+                  <c:v>58577.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107438</c:v>
+                  <c:v>107438.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>66480</c:v>
+                  <c:v>66480.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>204302</c:v>
+                  <c:v>204302.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>333571</c:v>
+                  <c:v>333571.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>512276</c:v>
+                  <c:v>512276.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1094920</c:v>
+                  <c:v>1.09492E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2102100</c:v>
+                  <c:v>2.1021E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4084700</c:v>
+                  <c:v>4.0847E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7777260</c:v>
+                  <c:v>7.77726E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26097200</c:v>
+                  <c:v>2.60972E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50709400</c:v>
+                  <c:v>5.07094E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76291900</c:v>
+                  <c:v>7.62919E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>137391000</c:v>
+                  <c:v>1.37391E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250417000</c:v>
+                  <c:v>2.50417E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3700,82 +3712,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3787,82 +3799,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>92</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>816</c:v>
+                  <c:v>816.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>684</c:v>
+                  <c:v>684.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>24776</c:v>
+                  <c:v>24776.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1452</c:v>
+                  <c:v>1452.0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1836</c:v>
+                  <c:v>1836.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2848</c:v>
+                  <c:v>2848.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3572</c:v>
+                  <c:v>3572.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>52305</c:v>
+                  <c:v>52305.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>29403</c:v>
+                  <c:v>29403.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>44484</c:v>
+                  <c:v>44484.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>71131</c:v>
+                  <c:v>71131.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>101508</c:v>
+                  <c:v>101508.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>142824</c:v>
+                  <c:v>142824.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>236131</c:v>
+                  <c:v>236131.0</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>293518</c:v>
+                  <c:v>293518.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>418489</c:v>
+                  <c:v>418489.0</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>607794</c:v>
+                  <c:v>607794.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>727373</c:v>
+                  <c:v>727373.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1302790</c:v>
+                  <c:v>1.30279E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>469364</c:v>
+                  <c:v>469364.0</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1821350</c:v>
+                  <c:v>1.82135E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>980792</c:v>
+                  <c:v>980792.0</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1406840</c:v>
+                  <c:v>1.40684E6</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1857820</c:v>
+                  <c:v>1.85782E6</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>2650960</c:v>
+                  <c:v>2.65096E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3904,82 +3916,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3991,82 +4003,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>264</c:v>
+                  <c:v>264.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>396</c:v>
+                  <c:v>396.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>576</c:v>
+                  <c:v>576.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1004</c:v>
+                  <c:v>1004.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1572</c:v>
+                  <c:v>1572.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2236</c:v>
+                  <c:v>2236.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3628</c:v>
+                  <c:v>3628.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>26829</c:v>
+                  <c:v>26829.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>45425</c:v>
+                  <c:v>45425.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>80883</c:v>
+                  <c:v>80883.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>158994</c:v>
+                  <c:v>158994.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>317724</c:v>
+                  <c:v>317724.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>622512</c:v>
+                  <c:v>622512.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1226590</c:v>
+                  <c:v>1.22659E6</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>2433140</c:v>
+                  <c:v>2.43314E6</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4877550</c:v>
+                  <c:v>4.87755E6</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>9721900</c:v>
+                  <c:v>9.7219E6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>17846500</c:v>
+                  <c:v>1.78465E7</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>24192500</c:v>
+                  <c:v>2.41925E7</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>27404700</c:v>
+                  <c:v>2.74047E7</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>57176400</c:v>
+                  <c:v>5.71764E7</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>76641300</c:v>
+                  <c:v>7.66413E7</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>143156000</c:v>
+                  <c:v>1.43156E8</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>286863000</c:v>
+                  <c:v>2.86863E8</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>559201000</c:v>
+                  <c:v>5.59201E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4108,82 +4120,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>362</c:v>
+                  <c:v>362.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>512</c:v>
+                  <c:v>512.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>724</c:v>
+                  <c:v>724.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1024</c:v>
+                  <c:v>1024.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1448</c:v>
+                  <c:v>1448.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2048</c:v>
+                  <c:v>2048.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2896</c:v>
+                  <c:v>2896.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4096</c:v>
+                  <c:v>4096.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5793</c:v>
+                  <c:v>5793.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8192</c:v>
+                  <c:v>8192.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4195,82 +4207,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>192.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>336</c:v>
+                  <c:v>336.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>456</c:v>
+                  <c:v>456.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>592</c:v>
+                  <c:v>592.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>964</c:v>
+                  <c:v>964.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1408</c:v>
+                  <c:v>1408.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2444</c:v>
+                  <c:v>2444.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14966</c:v>
+                  <c:v>14966.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26169</c:v>
+                  <c:v>26169.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44500</c:v>
+                  <c:v>44500.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84595</c:v>
+                  <c:v>84595.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>167871</c:v>
+                  <c:v>167871.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>330231</c:v>
+                  <c:v>330231.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>647361</c:v>
+                  <c:v>647361.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1288800</c:v>
+                  <c:v>1.2888E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2570020</c:v>
+                  <c:v>2.57002E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5112610</c:v>
+                  <c:v>5.11261E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10049800</c:v>
+                  <c:v>1.00498E7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13852800</c:v>
+                  <c:v>1.38528E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9463410</c:v>
+                  <c:v>9.46341E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40634300</c:v>
+                  <c:v>4.06343E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48241400</c:v>
+                  <c:v>4.82414E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>85835600</c:v>
+                  <c:v>8.58356E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>169027000</c:v>
+                  <c:v>1.69027E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>302730000</c:v>
+                  <c:v>3.0273E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>571163000</c:v>
+                  <c:v>5.71163E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4285,13 +4297,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="490650880"/>
-        <c:axId val="491134792"/>
+        <c:axId val="-2141122576"/>
+        <c:axId val="-2141128752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="490650880"/>
+        <c:axId val="-2141122576"/>
         <c:scaling>
-          <c:logBase val="2"/>
+          <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4408,16 +4420,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491134792"/>
+        <c:crossAx val="-2141128752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="4"/>
-        <c:minorUnit val="4"/>
+        <c:majorUnit val="4.0"/>
+        <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="491134792"/>
+        <c:axId val="-2141128752"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4534,8 +4546,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490650880"/>
-        <c:crossesAt val="1"/>
+        <c:crossAx val="-2141122576"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6061,16 +6073,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>462</v>
       </c>
@@ -6087,7 +6101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>499637</v>
       </c>
@@ -6104,7 +6118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>12969</v>
       </c>
@@ -6121,7 +6135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>14619</v>
       </c>
@@ -6138,7 +6152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>17177</v>
       </c>
@@ -6155,7 +6169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>21219</v>
       </c>
@@ -6172,7 +6186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>25130</v>
       </c>
@@ -6189,7 +6203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>33066</v>
       </c>
@@ -6206,7 +6220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>47091</v>
       </c>
@@ -6223,7 +6237,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>55193</v>
       </c>
@@ -6240,7 +6254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>120945</v>
       </c>
@@ -6257,7 +6271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>119724</v>
       </c>
@@ -6274,7 +6288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>163334</v>
       </c>
@@ -6291,7 +6305,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>208643</v>
       </c>
@@ -6308,7 +6322,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>333745</v>
       </c>
@@ -6325,7 +6339,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>458238</v>
       </c>
@@ -6342,7 +6356,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>691812</v>
       </c>
@@ -6359,7 +6373,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>970926</v>
       </c>
@@ -6376,7 +6390,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1420930</v>
       </c>
@@ -6393,7 +6407,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1344560</v>
       </c>
@@ -6410,7 +6424,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2066550</v>
       </c>
@@ -6427,7 +6441,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1070740</v>
       </c>
@@ -6444,7 +6458,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1576650</v>
       </c>
@@ -6461,7 +6475,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2230900</v>
       </c>
@@ -6478,7 +6492,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3309100</v>
       </c>
@@ -6495,7 +6509,7 @@
         <v>5793</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4714960</v>
       </c>
@@ -6512,7 +6526,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>56</v>
       </c>
@@ -6529,7 +6543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>424</v>
       </c>
@@ -6546,7 +6560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>872</v>
       </c>
@@ -6563,7 +6577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>896</v>
       </c>
@@ -6580,7 +6594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>35034</v>
       </c>
@@ -6597,7 +6611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2012</v>
       </c>
@@ -6614,7 +6628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>3024</v>
       </c>
@@ -6631,7 +6645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>3700</v>
       </c>
@@ -6648,7 +6662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>18348</v>
       </c>
@@ -6665,7 +6679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>6736</v>
       </c>
@@ -6682,7 +6696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>10916</v>
       </c>
@@ -6699,7 +6713,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>17036</v>
       </c>
@@ -6716,7 +6730,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>31204</v>
       </c>
@@ -6733,7 +6747,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>34656</v>
       </c>
@@ -6750,7 +6764,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>49300</v>
       </c>
@@ -6767,7 +6781,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>74376</v>
       </c>
@@ -6784,7 +6798,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>104764</v>
       </c>
@@ -6801,7 +6815,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>147752</v>
       </c>
@@ -6818,7 +6832,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>221676</v>
       </c>
@@ -6835,7 +6849,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>312292</v>
       </c>
@@ -6852,7 +6866,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>476340</v>
       </c>
@@ -6869,7 +6883,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>673732</v>
       </c>
@@ -6886,7 +6900,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>1006000</v>
       </c>
@@ -6903,7 +6917,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>1424090</v>
       </c>
@@ -6920,7 +6934,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>1905310</v>
       </c>
@@ -6937,7 +6951,7 @@
         <v>5793</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2699150</v>
       </c>
@@ -6954,7 +6968,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>92</v>
       </c>
@@ -6971,7 +6985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>816</v>
       </c>
@@ -6988,7 +7002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>684</v>
       </c>
@@ -7005,7 +7019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>24776</v>
       </c>
@@ -7022,7 +7036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>1452</v>
       </c>
@@ -7039,7 +7053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>1836</v>
       </c>
@@ -7056,7 +7070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2848</v>
       </c>
@@ -7073,7 +7087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3572</v>
       </c>
@@ -7090,7 +7104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>52305</v>
       </c>
@@ -7107,7 +7121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>29403</v>
       </c>
@@ -7124,7 +7138,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44484</v>
       </c>
@@ -7141,7 +7155,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>71131</v>
       </c>
@@ -7158,7 +7172,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>101508</v>
       </c>
@@ -7175,7 +7189,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>142824</v>
       </c>
@@ -7192,7 +7206,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>236131</v>
       </c>
@@ -7209,7 +7223,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>293518</v>
       </c>
@@ -7226,7 +7240,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>418489</v>
       </c>
@@ -7243,7 +7257,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>607794</v>
       </c>
@@ -7260,7 +7274,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>727373</v>
       </c>
@@ -7277,7 +7291,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>1302790</v>
       </c>
@@ -7294,7 +7308,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>469364</v>
       </c>
@@ -7311,7 +7325,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>1821350</v>
       </c>
@@ -7328,7 +7342,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>980792</v>
       </c>
@@ -7345,7 +7359,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>1406840</v>
       </c>
@@ -7362,7 +7376,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>1857820</v>
       </c>
@@ -7379,7 +7393,7 @@
         <v>5793</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>2650960</v>
       </c>

</xml_diff>

<commit_message>
Greatly improved write-up; tried and failed to make testing more fair.
</commit_message>
<xml_diff>
--- a/chartsnstuff.xlsx
+++ b/chartsnstuff.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25680" windowHeight="16120"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12880" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CPUcounts" localSheetId="0">Sheet1!$A$1:$E$78</definedName>
+    <definedName name="CPUcounts_1" localSheetId="0">Sheet1!$A$1:$E$78</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,8 +34,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="CPUcounts" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="S:\cs2500\cs2500project1\CPUcounts.txt" tab="0" space="1" consecutive="1">
+  <connection id="1" name="CPUcounts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Volumes/TOSHIBA/cs2500/Assignments/Project 1/cs2500project1/CPUcounts.txt" tab="0" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -136,7 +136,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Data Sorting CPU Counts </a:t>
+              <a:t>Data Sorting CPU Clock Cycles </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -196,7 +196,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Mergesort Random</c:v>
+            <c:v>Merge Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -314,82 +314,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>462.0</c:v>
+                  <c:v>515.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>499637.0</c:v>
+                  <c:v>157409.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12969.0</c:v>
+                  <c:v>10645.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14619.0</c:v>
+                  <c:v>11850.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17177.0</c:v>
+                  <c:v>125235.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21219.0</c:v>
+                  <c:v>21890.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25130.0</c:v>
+                  <c:v>25560.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33066.0</c:v>
+                  <c:v>38210.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47091.0</c:v>
+                  <c:v>49510.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55193.0</c:v>
+                  <c:v>36395.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120945.0</c:v>
+                  <c:v>78500.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119724.0</c:v>
+                  <c:v>103760.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>163334.0</c:v>
+                  <c:v>60530.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>208643.0</c:v>
+                  <c:v>249760.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>333745.0</c:v>
+                  <c:v>328631.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>458238.0</c:v>
+                  <c:v>517450.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>691812.0</c:v>
+                  <c:v>629865.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>970926.0</c:v>
+                  <c:v>750323.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.42093E6</c:v>
+                  <c:v>633030.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.34456E6</c:v>
+                  <c:v>1.30348E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.06655E6</c:v>
+                  <c:v>1.82876E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.07074E6</c:v>
+                  <c:v>2.57526E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.57665E6</c:v>
+                  <c:v>3.6951E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2309E6</c:v>
+                  <c:v>4.86843E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3091E6</c:v>
+                  <c:v>7.23642E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.71496E6</c:v>
+                  <c:v>4.76644E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,7 +400,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Insertionsort Random</c:v>
+            <c:v>Insertion Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -518,82 +518,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>181.0</c:v>
+                  <c:v>1010.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>891.0</c:v>
+                  <c:v>1300.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1369.0</c:v>
+                  <c:v>2380.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2145.0</c:v>
+                  <c:v>2240.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2887.0</c:v>
+                  <c:v>3390.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4505.0</c:v>
+                  <c:v>3770.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7260.0</c:v>
+                  <c:v>5820.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11154.0</c:v>
+                  <c:v>5934.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17787.0</c:v>
+                  <c:v>12950.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25773.0</c:v>
+                  <c:v>41110.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55786.0</c:v>
+                  <c:v>28981.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92186.0</c:v>
+                  <c:v>85590.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184536.0</c:v>
+                  <c:v>81725.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313681.0</c:v>
+                  <c:v>248866.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>659818.0</c:v>
+                  <c:v>444779.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.21686E6</c:v>
+                  <c:v>859642.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.47503E6</c:v>
+                  <c:v>1.73936E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.01648E6</c:v>
+                  <c:v>3.36027E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.85969E6</c:v>
+                  <c:v>5.51319E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.29319E7</c:v>
+                  <c:v>1.01914E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.51453E7</c:v>
+                  <c:v>1.89171E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.6792E7</c:v>
+                  <c:v>2.89104E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.40761E7</c:v>
+                  <c:v>5.12854E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.156E7</c:v>
+                  <c:v>9.26128E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.60177E8</c:v>
+                  <c:v>1.75859E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.79019E8</c:v>
+                  <c:v>3.41286E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -604,7 +604,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Bubblesort Random</c:v>
+            <c:v>Bubble Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -722,82 +722,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>775.0</c:v>
+                  <c:v>990.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039.0</c:v>
+                  <c:v>1290.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1667.0</c:v>
+                  <c:v>3870.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2392.0</c:v>
+                  <c:v>2590.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3861.0</c:v>
+                  <c:v>4370.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6055.0</c:v>
+                  <c:v>3301.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9586.0</c:v>
+                  <c:v>5099.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17803.0</c:v>
+                  <c:v>10100.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28165.0</c:v>
+                  <c:v>14407.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51051.0</c:v>
+                  <c:v>32840.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96063.0</c:v>
+                  <c:v>64190.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>161667.0</c:v>
+                  <c:v>52680.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>321123.0</c:v>
+                  <c:v>426211.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>585832.0</c:v>
+                  <c:v>379134.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.14053E6</c:v>
+                  <c:v>871267.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.13779E6</c:v>
+                  <c:v>1.62747E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.17739E6</c:v>
+                  <c:v>2.79206E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.18676E6</c:v>
+                  <c:v>4.12675E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.30109E7</c:v>
+                  <c:v>9.16109E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.09664E7</c:v>
+                  <c:v>1.72479E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.71862E7</c:v>
+                  <c:v>2.77688E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.55411E7</c:v>
+                  <c:v>4.50644E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.07552E7</c:v>
+                  <c:v>8.53463E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.49668E8</c:v>
+                  <c:v>1.86628E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.66394E8</c:v>
+                  <c:v>3.36934E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.55069E8</c:v>
+                  <c:v>7.11565E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,7 +808,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Mergesort Presorted</c:v>
+            <c:v>Merge Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -926,82 +926,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>56.0</c:v>
+                  <c:v>605.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424.0</c:v>
+                  <c:v>12730.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>872.0</c:v>
+                  <c:v>12180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>896.0</c:v>
+                  <c:v>17460.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35034.0</c:v>
+                  <c:v>13569.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2012.0</c:v>
+                  <c:v>20880.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3024.0</c:v>
+                  <c:v>17868.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3700.0</c:v>
+                  <c:v>27788.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18348.0</c:v>
+                  <c:v>52420.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6736.0</c:v>
+                  <c:v>37009.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10916.0</c:v>
+                  <c:v>108670.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17036.0</c:v>
+                  <c:v>106706.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31204.0</c:v>
+                  <c:v>183860.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34656.0</c:v>
+                  <c:v>218780.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49300.0</c:v>
+                  <c:v>101780.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74376.0</c:v>
+                  <c:v>542980.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104764.0</c:v>
+                  <c:v>405701.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>147752.0</c:v>
+                  <c:v>888887.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>221676.0</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>312292.0</c:v>
+                  <c:v>740947.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>812840.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>476340.0</c:v>
+                  <c:v>1.5255E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>673732.0</c:v>
+                  <c:v>2.48638E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.006E6</c:v>
+                  <c:v>1.6068E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.42409E6</c:v>
+                  <c:v>4.3366E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.90531E6</c:v>
+                  <c:v>5.76134E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.69915E6</c:v>
+                  <c:v>8.04469E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,7 +1012,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Insertionsort Presorted</c:v>
+            <c:v>Insertion Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1130,82 +1130,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>308.0</c:v>
+                  <c:v>720.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152.0</c:v>
+                  <c:v>2080.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156.0</c:v>
+                  <c:v>3300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>176.0</c:v>
+                  <c:v>1409.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>196.0</c:v>
+                  <c:v>1510.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216.0</c:v>
+                  <c:v>2460.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240.0</c:v>
+                  <c:v>2030.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>284.0</c:v>
+                  <c:v>2350.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>352.0</c:v>
+                  <c:v>1930.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>428.0</c:v>
+                  <c:v>2410.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>556.0</c:v>
+                  <c:v>3090.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>720.0</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>948.0</c:v>
+                  <c:v>3332.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1296.0</c:v>
+                  <c:v>5530.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1708.0</c:v>
+                  <c:v>2021.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2380.0</c:v>
+                  <c:v>6661.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3328.0</c:v>
+                  <c:v>11320.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41262.0</c:v>
+                  <c:v>27920.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43047.0</c:v>
+                  <c:v>22630.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9176.0</c:v>
+                  <c:v>31290.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12928.0</c:v>
+                  <c:v>41660.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54357.0</c:v>
+                  <c:v>66816.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59876.0</c:v>
+                  <c:v>84610.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36336.0</c:v>
+                  <c:v>122667.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51352.0</c:v>
+                  <c:v>163950.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72816.0</c:v>
+                  <c:v>64980.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,7 +1216,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Bubblesort Presorted</c:v>
+            <c:v>Bubble Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1334,82 +1334,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>116.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236.0</c:v>
+                  <c:v>1614.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>392.0</c:v>
+                  <c:v>1819.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>440.0</c:v>
+                  <c:v>1680.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>552.0</c:v>
+                  <c:v>1659.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>748.0</c:v>
+                  <c:v>2770.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1048.0</c:v>
+                  <c:v>2654.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1680.0</c:v>
+                  <c:v>5710.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2836.0</c:v>
+                  <c:v>8180.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4768.0</c:v>
+                  <c:v>13040.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45847.0</c:v>
+                  <c:v>22790.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58577.0</c:v>
+                  <c:v>30285.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107438.0</c:v>
+                  <c:v>77540.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>66480.0</c:v>
+                  <c:v>342580.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>204302.0</c:v>
+                  <c:v>238261.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>333571.0</c:v>
+                  <c:v>639565.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>512276.0</c:v>
+                  <c:v>868334.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.09492E6</c:v>
+                  <c:v>1.75657E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1021E6</c:v>
+                  <c:v>3.31271E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.0847E6</c:v>
+                  <c:v>5.22685E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.77726E6</c:v>
+                  <c:v>1.05406E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.60972E7</c:v>
+                  <c:v>1.86754E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.07094E7</c:v>
+                  <c:v>3.01193E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.62919E7</c:v>
+                  <c:v>5.14554E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.37391E8</c:v>
+                  <c:v>9.91362E7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.50417E8</c:v>
+                  <c:v>1.59232E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1420,7 +1420,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Mergesort Reverse Sorted</c:v>
+            <c:v>Merge Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1538,82 +1538,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>92.0</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>816.0</c:v>
+                  <c:v>13710.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>684.0</c:v>
+                  <c:v>14870.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>24776.0</c:v>
+                  <c:v>17220.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1452.0</c:v>
+                  <c:v>17610.0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1836.0</c:v>
+                  <c:v>15238.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2848.0</c:v>
+                  <c:v>45640.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3572.0</c:v>
+                  <c:v>41440.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>52305.0</c:v>
+                  <c:v>47010.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>29403.0</c:v>
+                  <c:v>32880.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>44484.0</c:v>
+                  <c:v>67180.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>71131.0</c:v>
+                  <c:v>88620.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>101508.0</c:v>
+                  <c:v>145944.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>142824.0</c:v>
+                  <c:v>79812.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>236131.0</c:v>
+                  <c:v>461002.0</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>293518.0</c:v>
+                  <c:v>367880.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>418489.0</c:v>
+                  <c:v>287345.0</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>607794.0</c:v>
+                  <c:v>528981.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>727373.0</c:v>
+                  <c:v>726737.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1.30279E6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>469364.0</c:v>
+                  <c:v>1.35405E6</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00E+00">
+                  <c:v>1.36756E6</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.82135E6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>980792.0</c:v>
+                  <c:v>2.42584E6</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>3.39491E6</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.40684E6</c:v>
+                  <c:v>4.50512E6</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1.85782E6</c:v>
+                  <c:v>6.07704E6</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>2.65096E6</c:v>
+                  <c:v>7.56442E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,7 +1624,7 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Insertionsort Reverse Sorted</c:v>
+            <c:v>Insertion Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1742,82 +1742,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>24.0</c:v>
+                  <c:v>1060.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>264.0</c:v>
+                  <c:v>1513.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>396.0</c:v>
+                  <c:v>2390.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>576.0</c:v>
+                  <c:v>3300.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1004.0</c:v>
+                  <c:v>3301.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1572.0</c:v>
+                  <c:v>6660.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2236.0</c:v>
+                  <c:v>7310.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3628.0</c:v>
+                  <c:v>7115.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>26829.0</c:v>
+                  <c:v>21480.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>45425.0</c:v>
+                  <c:v>25565.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>80883.0</c:v>
+                  <c:v>80908.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>158994.0</c:v>
+                  <c:v>128710.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>317724.0</c:v>
+                  <c:v>113736.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>622512.0</c:v>
+                  <c:v>254320.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1.22659E6</c:v>
+                  <c:v>1.2085E6</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>2.43314E6</c:v>
+                  <c:v>1.89351E6</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4.87755E6</c:v>
+                  <c:v>3.54852E6</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>9.7219E6</c:v>
+                  <c:v>5.14306E6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>1.78465E7</c:v>
+                  <c:v>1.10327E7</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>2.41925E7</c:v>
+                  <c:v>1.89473E7</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>2.74047E7</c:v>
+                  <c:v>3.16328E7</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>5.71764E7</c:v>
+                  <c:v>5.04607E7</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>7.66413E7</c:v>
+                  <c:v>9.77571E7</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.43156E8</c:v>
+                  <c:v>1.62686E8</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>2.86863E8</c:v>
+                  <c:v>3.33139E8</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>5.59201E8</c:v>
+                  <c:v>6.4879E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1828,7 +1828,7 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>Bubblesort Reverse Sorted</c:v>
+            <c:v>Bubble Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1946,82 +1946,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>192.0</c:v>
+                  <c:v>1010.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>336.0</c:v>
+                  <c:v>2320.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>456.0</c:v>
+                  <c:v>1885.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>592.0</c:v>
+                  <c:v>2780.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>964.0</c:v>
+                  <c:v>3560.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1408.0</c:v>
+                  <c:v>3652.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2444.0</c:v>
+                  <c:v>7850.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14966.0</c:v>
+                  <c:v>12900.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26169.0</c:v>
+                  <c:v>21350.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44500.0</c:v>
+                  <c:v>47690.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84595.0</c:v>
+                  <c:v>84840.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>167871.0</c:v>
+                  <c:v>371329.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>330231.0</c:v>
+                  <c:v>164249.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>647361.0</c:v>
+                  <c:v>679613.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2888E6</c:v>
+                  <c:v>1.16808E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.57002E6</c:v>
+                  <c:v>2.20234E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.11261E6</c:v>
+                  <c:v>3.21468E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.00498E7</c:v>
+                  <c:v>6.59037E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.38528E7</c:v>
+                  <c:v>1.23139E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.46341E6</c:v>
+                  <c:v>2.31682E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.06343E7</c:v>
+                  <c:v>3.37831E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.82414E7</c:v>
+                  <c:v>6.92515E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.58356E7</c:v>
+                  <c:v>1.17393E8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.69027E8</c:v>
+                  <c:v>1.90406E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.0273E8</c:v>
+                  <c:v>3.84898E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.71163E8</c:v>
+                  <c:v>8.03016E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2036,11 +2036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140950224"/>
-        <c:axId val="-2140958752"/>
+        <c:axId val="-2126656224"/>
+        <c:axId val="-2126647696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140950224"/>
+        <c:axId val="-2126656224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,12 +2158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140958752"/>
+        <c:crossAx val="-2126647696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140958752"/>
+        <c:axId val="-2126647696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,8 +2204,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>CPU counts</a:t>
+                  <a:t>CPU Clock</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Cycles</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2276,7 +2281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140950224"/>
+        <c:crossAx val="-2126656224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2401,7 +2406,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Data Sorting CPU Counts (logarithmic scale)</a:t>
+              <a:t>Data Sorting CPU Clock Cycles (logarithmic scale)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2457,7 +2462,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Mergesort Random</c:v>
+            <c:v>Merge Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2575,82 +2580,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>462.0</c:v>
+                  <c:v>515.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>499637.0</c:v>
+                  <c:v>157409.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12969.0</c:v>
+                  <c:v>10645.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14619.0</c:v>
+                  <c:v>11850.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17177.0</c:v>
+                  <c:v>125235.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21219.0</c:v>
+                  <c:v>21890.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25130.0</c:v>
+                  <c:v>25560.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33066.0</c:v>
+                  <c:v>38210.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47091.0</c:v>
+                  <c:v>49510.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55193.0</c:v>
+                  <c:v>36395.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120945.0</c:v>
+                  <c:v>78500.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119724.0</c:v>
+                  <c:v>103760.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>163334.0</c:v>
+                  <c:v>60530.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>208643.0</c:v>
+                  <c:v>249760.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>333745.0</c:v>
+                  <c:v>328631.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>458238.0</c:v>
+                  <c:v>517450.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>691812.0</c:v>
+                  <c:v>629865.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>970926.0</c:v>
+                  <c:v>750323.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.42093E6</c:v>
+                  <c:v>633030.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.34456E6</c:v>
+                  <c:v>1.30348E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.06655E6</c:v>
+                  <c:v>1.82876E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.07074E6</c:v>
+                  <c:v>2.57526E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.57665E6</c:v>
+                  <c:v>3.6951E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2309E6</c:v>
+                  <c:v>4.86843E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3091E6</c:v>
+                  <c:v>7.23642E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.71496E6</c:v>
+                  <c:v>4.76644E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2661,7 +2666,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Insertionsort Random</c:v>
+            <c:v>Insertion Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2779,82 +2784,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>181.0</c:v>
+                  <c:v>1010.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>891.0</c:v>
+                  <c:v>1300.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1369.0</c:v>
+                  <c:v>2380.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2145.0</c:v>
+                  <c:v>2240.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2887.0</c:v>
+                  <c:v>3390.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4505.0</c:v>
+                  <c:v>3770.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7260.0</c:v>
+                  <c:v>5820.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11154.0</c:v>
+                  <c:v>5934.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17787.0</c:v>
+                  <c:v>12950.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25773.0</c:v>
+                  <c:v>41110.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55786.0</c:v>
+                  <c:v>28981.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92186.0</c:v>
+                  <c:v>85590.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184536.0</c:v>
+                  <c:v>81725.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>313681.0</c:v>
+                  <c:v>248866.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>659818.0</c:v>
+                  <c:v>444779.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.21686E6</c:v>
+                  <c:v>859642.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.47503E6</c:v>
+                  <c:v>1.73936E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.01648E6</c:v>
+                  <c:v>3.36027E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.85969E6</c:v>
+                  <c:v>5.51319E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.29319E7</c:v>
+                  <c:v>1.01914E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.51453E7</c:v>
+                  <c:v>1.89171E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.6792E7</c:v>
+                  <c:v>2.89104E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.40761E7</c:v>
+                  <c:v>5.12854E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.156E7</c:v>
+                  <c:v>9.26128E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.60177E8</c:v>
+                  <c:v>1.75859E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.79019E8</c:v>
+                  <c:v>3.41286E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2865,7 +2870,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Bubblesort Random</c:v>
+            <c:v>Bubble Sort Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2983,82 +2988,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>775.0</c:v>
+                  <c:v>990.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039.0</c:v>
+                  <c:v>1290.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1667.0</c:v>
+                  <c:v>3870.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2392.0</c:v>
+                  <c:v>2590.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3861.0</c:v>
+                  <c:v>4370.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6055.0</c:v>
+                  <c:v>3301.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9586.0</c:v>
+                  <c:v>5099.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17803.0</c:v>
+                  <c:v>10100.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28165.0</c:v>
+                  <c:v>14407.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51051.0</c:v>
+                  <c:v>32840.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96063.0</c:v>
+                  <c:v>64190.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>161667.0</c:v>
+                  <c:v>52680.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>321123.0</c:v>
+                  <c:v>426211.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>585832.0</c:v>
+                  <c:v>379134.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.14053E6</c:v>
+                  <c:v>871267.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.13779E6</c:v>
+                  <c:v>1.62747E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.17739E6</c:v>
+                  <c:v>2.79206E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.18676E6</c:v>
+                  <c:v>4.12675E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.30109E7</c:v>
+                  <c:v>9.16109E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.09664E7</c:v>
+                  <c:v>1.72479E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.71862E7</c:v>
+                  <c:v>2.77688E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.55411E7</c:v>
+                  <c:v>4.50644E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.07552E7</c:v>
+                  <c:v>8.53463E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.49668E8</c:v>
+                  <c:v>1.86628E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.66394E8</c:v>
+                  <c:v>3.36934E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.55069E8</c:v>
+                  <c:v>7.11565E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3069,7 +3074,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Mergesort Presorted</c:v>
+            <c:v>Merge Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3187,82 +3192,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>56.0</c:v>
+                  <c:v>605.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424.0</c:v>
+                  <c:v>12730.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>872.0</c:v>
+                  <c:v>12180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>896.0</c:v>
+                  <c:v>17460.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35034.0</c:v>
+                  <c:v>13569.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2012.0</c:v>
+                  <c:v>20880.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3024.0</c:v>
+                  <c:v>17868.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3700.0</c:v>
+                  <c:v>27788.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18348.0</c:v>
+                  <c:v>52420.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6736.0</c:v>
+                  <c:v>37009.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10916.0</c:v>
+                  <c:v>108670.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17036.0</c:v>
+                  <c:v>106706.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31204.0</c:v>
+                  <c:v>183860.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34656.0</c:v>
+                  <c:v>218780.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49300.0</c:v>
+                  <c:v>101780.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74376.0</c:v>
+                  <c:v>542980.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104764.0</c:v>
+                  <c:v>405701.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>147752.0</c:v>
+                  <c:v>888887.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>221676.0</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>312292.0</c:v>
+                  <c:v>740947.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>812840.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>476340.0</c:v>
+                  <c:v>1.5255E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>673732.0</c:v>
+                  <c:v>2.48638E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.006E6</c:v>
+                  <c:v>1.6068E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.42409E6</c:v>
+                  <c:v>4.3366E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.90531E6</c:v>
+                  <c:v>5.76134E6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.69915E6</c:v>
+                  <c:v>8.04469E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3273,7 +3278,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Insertionsort Presorted</c:v>
+            <c:v>Insertion Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3391,82 +3396,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>308.0</c:v>
+                  <c:v>720.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152.0</c:v>
+                  <c:v>2080.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156.0</c:v>
+                  <c:v>3300.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>176.0</c:v>
+                  <c:v>1409.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>196.0</c:v>
+                  <c:v>1510.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216.0</c:v>
+                  <c:v>2460.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240.0</c:v>
+                  <c:v>2030.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>284.0</c:v>
+                  <c:v>2350.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>352.0</c:v>
+                  <c:v>1930.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>428.0</c:v>
+                  <c:v>2410.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>556.0</c:v>
+                  <c:v>3090.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>720.0</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>948.0</c:v>
+                  <c:v>3332.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1296.0</c:v>
+                  <c:v>5530.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1708.0</c:v>
+                  <c:v>2021.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2380.0</c:v>
+                  <c:v>6661.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3328.0</c:v>
+                  <c:v>11320.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41262.0</c:v>
+                  <c:v>27920.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43047.0</c:v>
+                  <c:v>22630.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9176.0</c:v>
+                  <c:v>31290.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12928.0</c:v>
+                  <c:v>41660.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54357.0</c:v>
+                  <c:v>66816.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59876.0</c:v>
+                  <c:v>84610.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36336.0</c:v>
+                  <c:v>122667.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51352.0</c:v>
+                  <c:v>163950.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72816.0</c:v>
+                  <c:v>64980.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3477,7 +3482,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Bubblesort Presorted</c:v>
+            <c:v>Bubble Sort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3595,82 +3600,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>116.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236.0</c:v>
+                  <c:v>1614.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>392.0</c:v>
+                  <c:v>1819.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>440.0</c:v>
+                  <c:v>1680.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>552.0</c:v>
+                  <c:v>1659.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>748.0</c:v>
+                  <c:v>2770.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1048.0</c:v>
+                  <c:v>2654.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1680.0</c:v>
+                  <c:v>5710.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2836.0</c:v>
+                  <c:v>8180.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4768.0</c:v>
+                  <c:v>13040.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45847.0</c:v>
+                  <c:v>22790.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58577.0</c:v>
+                  <c:v>30285.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107438.0</c:v>
+                  <c:v>77540.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>66480.0</c:v>
+                  <c:v>342580.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>204302.0</c:v>
+                  <c:v>238261.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>333571.0</c:v>
+                  <c:v>639565.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>512276.0</c:v>
+                  <c:v>868334.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.09492E6</c:v>
+                  <c:v>1.75657E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1021E6</c:v>
+                  <c:v>3.31271E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.0847E6</c:v>
+                  <c:v>5.22685E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.77726E6</c:v>
+                  <c:v>1.05406E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.60972E7</c:v>
+                  <c:v>1.86754E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.07094E7</c:v>
+                  <c:v>3.01193E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.62919E7</c:v>
+                  <c:v>5.14554E7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.37391E8</c:v>
+                  <c:v>9.91362E7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.50417E8</c:v>
+                  <c:v>1.59232E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3681,7 +3686,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Mergesort Reverse Sorted</c:v>
+            <c:v>Merge Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3799,82 +3804,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>92.0</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>816.0</c:v>
+                  <c:v>13710.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>684.0</c:v>
+                  <c:v>14870.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>24776.0</c:v>
+                  <c:v>17220.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1452.0</c:v>
+                  <c:v>17610.0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1836.0</c:v>
+                  <c:v>15238.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2848.0</c:v>
+                  <c:v>45640.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3572.0</c:v>
+                  <c:v>41440.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>52305.0</c:v>
+                  <c:v>47010.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>29403.0</c:v>
+                  <c:v>32880.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>44484.0</c:v>
+                  <c:v>67180.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>71131.0</c:v>
+                  <c:v>88620.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>101508.0</c:v>
+                  <c:v>145944.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>142824.0</c:v>
+                  <c:v>79812.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>236131.0</c:v>
+                  <c:v>461002.0</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>293518.0</c:v>
+                  <c:v>367880.0</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>418489.0</c:v>
+                  <c:v>287345.0</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>607794.0</c:v>
+                  <c:v>528981.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>727373.0</c:v>
+                  <c:v>726737.0</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>1.30279E6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>469364.0</c:v>
+                  <c:v>1.35405E6</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00E+00">
+                  <c:v>1.36756E6</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.82135E6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>980792.0</c:v>
+                  <c:v>2.42584E6</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>3.39491E6</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.40684E6</c:v>
+                  <c:v>4.50512E6</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>1.85782E6</c:v>
+                  <c:v>6.07704E6</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>2.65096E6</c:v>
+                  <c:v>7.56442E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3885,7 +3890,7 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Insertionsort Reverse Sorted</c:v>
+            <c:v>Insertion Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -4003,82 +4008,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>24.0</c:v>
+                  <c:v>1060.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>264.0</c:v>
+                  <c:v>1513.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>396.0</c:v>
+                  <c:v>2390.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>576.0</c:v>
+                  <c:v>3300.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1004.0</c:v>
+                  <c:v>3301.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1572.0</c:v>
+                  <c:v>6660.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>2236.0</c:v>
+                  <c:v>7310.0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>3628.0</c:v>
+                  <c:v>7115.0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>26829.0</c:v>
+                  <c:v>21480.0</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>45425.0</c:v>
+                  <c:v>25565.0</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>80883.0</c:v>
+                  <c:v>80908.0</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>158994.0</c:v>
+                  <c:v>128710.0</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>317724.0</c:v>
+                  <c:v>113736.0</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>622512.0</c:v>
+                  <c:v>254320.0</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>1.22659E6</c:v>
+                  <c:v>1.2085E6</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>2.43314E6</c:v>
+                  <c:v>1.89351E6</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>4.87755E6</c:v>
+                  <c:v>3.54852E6</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>9.7219E6</c:v>
+                  <c:v>5.14306E6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>1.78465E7</c:v>
+                  <c:v>1.10327E7</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>2.41925E7</c:v>
+                  <c:v>1.89473E7</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>2.74047E7</c:v>
+                  <c:v>3.16328E7</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>5.71764E7</c:v>
+                  <c:v>5.04607E7</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>7.66413E7</c:v>
+                  <c:v>9.77571E7</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>1.43156E8</c:v>
+                  <c:v>1.62686E8</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>2.86863E8</c:v>
+                  <c:v>3.33139E8</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>5.59201E8</c:v>
+                  <c:v>6.4879E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4089,7 +4094,7 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>Bubblesort Reverse Sorted</c:v>
+            <c:v>Bubble Sort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -4207,82 +4212,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>192.0</c:v>
+                  <c:v>1010.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>336.0</c:v>
+                  <c:v>2320.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>456.0</c:v>
+                  <c:v>1885.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>592.0</c:v>
+                  <c:v>2780.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>964.0</c:v>
+                  <c:v>3560.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1408.0</c:v>
+                  <c:v>3652.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2444.0</c:v>
+                  <c:v>7850.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14966.0</c:v>
+                  <c:v>12900.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26169.0</c:v>
+                  <c:v>21350.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44500.0</c:v>
+                  <c:v>47690.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84595.0</c:v>
+                  <c:v>84840.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>167871.0</c:v>
+                  <c:v>371329.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>330231.0</c:v>
+                  <c:v>164249.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>647361.0</c:v>
+                  <c:v>679613.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2888E6</c:v>
+                  <c:v>1.16808E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.57002E6</c:v>
+                  <c:v>2.20234E6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.11261E6</c:v>
+                  <c:v>3.21468E6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.00498E7</c:v>
+                  <c:v>6.59037E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.38528E7</c:v>
+                  <c:v>1.23139E7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.46341E6</c:v>
+                  <c:v>2.31682E7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.06343E7</c:v>
+                  <c:v>3.37831E7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.82414E7</c:v>
+                  <c:v>6.92515E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.58356E7</c:v>
+                  <c:v>1.17393E8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.69027E8</c:v>
+                  <c:v>1.90406E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.0273E8</c:v>
+                  <c:v>3.84898E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.71163E8</c:v>
+                  <c:v>8.03016E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4297,11 +4302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141122576"/>
-        <c:axId val="-2141128752"/>
+        <c:axId val="2146711408"/>
+        <c:axId val="2146705232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141122576"/>
+        <c:axId val="2146711408"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4420,14 +4425,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141128752"/>
+        <c:crossAx val="2146705232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141128752"/>
+        <c:axId val="2146705232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4473,7 +4478,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> counts</a:t>
+                  <a:t> Clock Cycles</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -4546,7 +4551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2141122576"/>
+        <c:crossAx val="2146711408"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5744,15 +5749,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>184660</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66231</xdr:rowOff>
+      <xdr:colOff>30238</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>489460</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>175434</xdr:rowOff>
+      <xdr:colOff>335038</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109204</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5805,7 +5810,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="CPUcounts" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="CPUcounts_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6073,26 +6078,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>462</v>
+        <v>515</v>
       </c>
       <c r="B1" s="1">
-        <v>181</v>
+        <v>1010</v>
       </c>
       <c r="C1" s="1">
-        <v>775</v>
+        <v>990</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -6103,13 +6106,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>499637</v>
+        <v>157409</v>
       </c>
       <c r="B2" s="1">
-        <v>891</v>
+        <v>1300</v>
       </c>
       <c r="C2" s="1">
-        <v>1039</v>
+        <v>1290</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -6120,13 +6123,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>12969</v>
+        <v>10645</v>
       </c>
       <c r="B3" s="1">
-        <v>1369</v>
+        <v>2380</v>
       </c>
       <c r="C3" s="1">
-        <v>1667</v>
+        <v>3870</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -6137,13 +6140,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>14619</v>
+        <v>11850</v>
       </c>
       <c r="B4" s="1">
-        <v>2145</v>
+        <v>2240</v>
       </c>
       <c r="C4" s="1">
-        <v>2392</v>
+        <v>2590</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -6154,13 +6157,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>17177</v>
+        <v>125235</v>
       </c>
       <c r="B5" s="1">
-        <v>2887</v>
+        <v>3390</v>
       </c>
       <c r="C5" s="1">
-        <v>3861</v>
+        <v>4370</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -6171,13 +6174,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>21219</v>
+        <v>21890</v>
       </c>
       <c r="B6" s="1">
-        <v>4505</v>
+        <v>3770</v>
       </c>
       <c r="C6" s="1">
-        <v>6055</v>
+        <v>3301</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -6188,13 +6191,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>25130</v>
+        <v>25560</v>
       </c>
       <c r="B7" s="1">
-        <v>7260</v>
+        <v>5820</v>
       </c>
       <c r="C7" s="1">
-        <v>9586</v>
+        <v>5099</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -6205,13 +6208,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>33066</v>
+        <v>38210</v>
       </c>
       <c r="B8" s="1">
-        <v>11154</v>
+        <v>5934</v>
       </c>
       <c r="C8" s="1">
-        <v>17803</v>
+        <v>10100</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -6222,13 +6225,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>47091</v>
+        <v>49510</v>
       </c>
       <c r="B9" s="1">
-        <v>17787</v>
+        <v>12950</v>
       </c>
       <c r="C9" s="1">
-        <v>28165</v>
+        <v>14407</v>
       </c>
       <c r="D9">
         <v>9</v>
@@ -6239,13 +6242,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>55193</v>
+        <v>36395</v>
       </c>
       <c r="B10" s="1">
-        <v>25773</v>
+        <v>41110</v>
       </c>
       <c r="C10" s="1">
-        <v>51051</v>
+        <v>32840</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -6256,13 +6259,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>120945</v>
+        <v>78500</v>
       </c>
       <c r="B11" s="1">
-        <v>55786</v>
+        <v>28981</v>
       </c>
       <c r="C11" s="1">
-        <v>96063</v>
+        <v>64190</v>
       </c>
       <c r="D11">
         <v>11</v>
@@ -6273,13 +6276,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>119724</v>
+        <v>103760</v>
       </c>
       <c r="B12" s="1">
-        <v>92186</v>
+        <v>85590</v>
       </c>
       <c r="C12" s="1">
-        <v>161667</v>
+        <v>52680</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -6290,13 +6293,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>163334</v>
+        <v>60530</v>
       </c>
       <c r="B13" s="1">
-        <v>184536</v>
+        <v>81725</v>
       </c>
       <c r="C13" s="1">
-        <v>321123</v>
+        <v>426211</v>
       </c>
       <c r="D13">
         <v>13</v>
@@ -6307,13 +6310,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>208643</v>
+        <v>249760</v>
       </c>
       <c r="B14" s="1">
-        <v>313681</v>
+        <v>248866</v>
       </c>
       <c r="C14" s="1">
-        <v>585832</v>
+        <v>379134</v>
       </c>
       <c r="D14">
         <v>14</v>
@@ -6324,13 +6327,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>333745</v>
+        <v>328631</v>
       </c>
       <c r="B15" s="1">
-        <v>659818</v>
+        <v>444779</v>
       </c>
       <c r="C15" s="1">
-        <v>1140530</v>
+        <v>871267</v>
       </c>
       <c r="D15">
         <v>15</v>
@@ -6341,13 +6344,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>458238</v>
+        <v>517450</v>
       </c>
       <c r="B16" s="1">
-        <v>1216860</v>
+        <v>859642</v>
       </c>
       <c r="C16" s="1">
-        <v>2137790</v>
+        <v>1627470</v>
       </c>
       <c r="D16">
         <v>16</v>
@@ -6358,13 +6361,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>691812</v>
+        <v>629865</v>
       </c>
       <c r="B17" s="1">
-        <v>2475030</v>
+        <v>1739360</v>
       </c>
       <c r="C17" s="1">
-        <v>4177390</v>
+        <v>2792060</v>
       </c>
       <c r="D17">
         <v>17</v>
@@ -6375,13 +6378,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>970926</v>
+        <v>750323</v>
       </c>
       <c r="B18" s="1">
-        <v>5016480</v>
+        <v>3360270</v>
       </c>
       <c r="C18" s="1">
-        <v>8186760</v>
+        <v>4126750</v>
       </c>
       <c r="D18">
         <v>18</v>
@@ -6392,13 +6395,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>1420930</v>
+        <v>633030</v>
       </c>
       <c r="B19" s="1">
-        <v>9859690</v>
+        <v>5513190</v>
       </c>
       <c r="C19" s="1">
-        <v>13010900</v>
+        <v>9161090</v>
       </c>
       <c r="D19">
         <v>19</v>
@@ -6409,13 +6412,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>1344560</v>
+        <v>1303480</v>
       </c>
       <c r="B20" s="1">
-        <v>12931900</v>
+        <v>10191400</v>
       </c>
       <c r="C20" s="1">
-        <v>20966400</v>
+        <v>17247900</v>
       </c>
       <c r="D20">
         <v>20</v>
@@ -6426,13 +6429,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2066550</v>
+        <v>1828760</v>
       </c>
       <c r="B21" s="1">
-        <v>25145300</v>
+        <v>18917100</v>
       </c>
       <c r="C21" s="1">
-        <v>27186200</v>
+        <v>27768800</v>
       </c>
       <c r="D21">
         <v>21</v>
@@ -6443,13 +6446,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>1070740</v>
+        <v>2575260</v>
       </c>
       <c r="B22" s="1">
-        <v>26792000</v>
+        <v>28910400</v>
       </c>
       <c r="C22" s="1">
-        <v>55541100</v>
+        <v>45064400</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -6460,13 +6463,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>1576650</v>
+        <v>3695100</v>
       </c>
       <c r="B23" s="1">
-        <v>44076100</v>
+        <v>51285400</v>
       </c>
       <c r="C23" s="1">
-        <v>70755200</v>
+        <v>85346300</v>
       </c>
       <c r="D23">
         <v>23</v>
@@ -6477,13 +6480,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>2230900</v>
+        <v>4868430</v>
       </c>
       <c r="B24" s="1">
-        <v>81560000</v>
+        <v>92612800</v>
       </c>
       <c r="C24" s="1">
-        <v>149668000</v>
+        <v>186628000</v>
       </c>
       <c r="D24">
         <v>24</v>
@@ -6494,13 +6497,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>3309100</v>
+        <v>7236420</v>
       </c>
       <c r="B25" s="1">
-        <v>160177000</v>
+        <v>175859000</v>
       </c>
       <c r="C25" s="1">
-        <v>266394000</v>
+        <v>336934000</v>
       </c>
       <c r="D25">
         <v>25</v>
@@ -6511,13 +6514,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>4714960</v>
+        <v>4766440</v>
       </c>
       <c r="B26" s="1">
-        <v>279019000</v>
+        <v>341286000</v>
       </c>
       <c r="C26" s="1">
-        <v>555069000</v>
+        <v>711565000</v>
       </c>
       <c r="D26">
         <v>26</v>
@@ -6528,13 +6531,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>56</v>
+        <v>605</v>
       </c>
       <c r="B27" s="1">
-        <v>308</v>
+        <v>720</v>
       </c>
       <c r="C27" s="1">
-        <v>116</v>
+        <v>1000</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -6545,13 +6548,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>424</v>
+        <v>12730</v>
       </c>
       <c r="B28" s="1">
-        <v>152</v>
+        <v>2080</v>
       </c>
       <c r="C28" s="1">
-        <v>236</v>
+        <v>1614</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -6562,13 +6565,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>872</v>
+        <v>12180</v>
       </c>
       <c r="B29" s="1">
-        <v>156</v>
+        <v>3300</v>
       </c>
       <c r="C29" s="1">
-        <v>392</v>
+        <v>1819</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -6579,13 +6582,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>896</v>
+        <v>17460</v>
       </c>
       <c r="B30" s="1">
-        <v>176</v>
+        <v>1409</v>
       </c>
       <c r="C30" s="1">
-        <v>440</v>
+        <v>1680</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -6596,13 +6599,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>35034</v>
+        <v>13569</v>
       </c>
       <c r="B31" s="1">
-        <v>196</v>
+        <v>1510</v>
       </c>
       <c r="C31" s="1">
-        <v>552</v>
+        <v>1659</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -6613,13 +6616,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>2012</v>
+        <v>20880</v>
       </c>
       <c r="B32" s="1">
-        <v>216</v>
+        <v>2460</v>
       </c>
       <c r="C32" s="1">
-        <v>748</v>
+        <v>2770</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -6630,13 +6633,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>3024</v>
+        <v>17868</v>
       </c>
       <c r="B33" s="1">
-        <v>240</v>
+        <v>2030</v>
       </c>
       <c r="C33" s="1">
-        <v>1048</v>
+        <v>2654</v>
       </c>
       <c r="D33">
         <v>7</v>
@@ -6647,13 +6650,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>3700</v>
+        <v>27788</v>
       </c>
       <c r="B34" s="1">
-        <v>284</v>
+        <v>2350</v>
       </c>
       <c r="C34" s="1">
-        <v>1680</v>
+        <v>5710</v>
       </c>
       <c r="D34">
         <v>8</v>
@@ -6664,13 +6667,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>18348</v>
+        <v>52420</v>
       </c>
       <c r="B35" s="1">
-        <v>352</v>
+        <v>1930</v>
       </c>
       <c r="C35" s="1">
-        <v>2836</v>
+        <v>8180</v>
       </c>
       <c r="D35">
         <v>9</v>
@@ -6681,13 +6684,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>6736</v>
+        <v>37009</v>
       </c>
       <c r="B36" s="1">
-        <v>428</v>
+        <v>2410</v>
       </c>
       <c r="C36" s="1">
-        <v>4768</v>
+        <v>13040</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -6698,13 +6701,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>10916</v>
+        <v>108670</v>
       </c>
       <c r="B37" s="1">
-        <v>556</v>
+        <v>3090</v>
       </c>
       <c r="C37" s="1">
-        <v>45847</v>
+        <v>22790</v>
       </c>
       <c r="D37">
         <v>11</v>
@@ -6715,13 +6718,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>17036</v>
+        <v>106706</v>
       </c>
       <c r="B38" s="1">
-        <v>720</v>
+        <v>3500</v>
       </c>
       <c r="C38" s="1">
-        <v>58577</v>
+        <v>30285</v>
       </c>
       <c r="D38">
         <v>12</v>
@@ -6732,13 +6735,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>31204</v>
+        <v>183860</v>
       </c>
       <c r="B39" s="1">
-        <v>948</v>
+        <v>3332</v>
       </c>
       <c r="C39" s="1">
-        <v>107438</v>
+        <v>77540</v>
       </c>
       <c r="D39">
         <v>13</v>
@@ -6749,13 +6752,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>34656</v>
+        <v>218780</v>
       </c>
       <c r="B40" s="1">
-        <v>1296</v>
+        <v>5530</v>
       </c>
       <c r="C40" s="1">
-        <v>66480</v>
+        <v>342580</v>
       </c>
       <c r="D40">
         <v>14</v>
@@ -6766,13 +6769,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>49300</v>
+        <v>101780</v>
       </c>
       <c r="B41" s="1">
-        <v>1708</v>
+        <v>2021</v>
       </c>
       <c r="C41" s="1">
-        <v>204302</v>
+        <v>238261</v>
       </c>
       <c r="D41">
         <v>15</v>
@@ -6783,13 +6786,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>74376</v>
+        <v>542980</v>
       </c>
       <c r="B42" s="1">
-        <v>2380</v>
+        <v>6661</v>
       </c>
       <c r="C42" s="1">
-        <v>333571</v>
+        <v>639565</v>
       </c>
       <c r="D42">
         <v>16</v>
@@ -6800,13 +6803,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>104764</v>
+        <v>405701</v>
       </c>
       <c r="B43" s="1">
-        <v>3328</v>
+        <v>11320</v>
       </c>
       <c r="C43">
-        <v>512276</v>
+        <v>868334</v>
       </c>
       <c r="D43">
         <v>17</v>
@@ -6817,13 +6820,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>147752</v>
+        <v>888887</v>
       </c>
       <c r="B44" s="1">
-        <v>41262</v>
+        <v>27920</v>
       </c>
       <c r="C44" s="1">
-        <v>1094920</v>
+        <v>1756570</v>
       </c>
       <c r="D44">
         <v>18</v>
@@ -6834,13 +6837,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>221676</v>
+        <v>740947</v>
       </c>
       <c r="B45" s="1">
-        <v>43047</v>
+        <v>22630</v>
       </c>
       <c r="C45" s="1">
-        <v>2102100</v>
+        <v>3312710</v>
       </c>
       <c r="D45">
         <v>19</v>
@@ -6850,14 +6853,14 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>312292</v>
+      <c r="A46" s="1">
+        <v>812840</v>
       </c>
       <c r="B46" s="1">
-        <v>9176</v>
+        <v>31290</v>
       </c>
       <c r="C46" s="1">
-        <v>4084700</v>
+        <v>5226850</v>
       </c>
       <c r="D46">
         <v>20</v>
@@ -6868,13 +6871,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>476340</v>
+        <v>1525500</v>
       </c>
       <c r="B47" s="1">
-        <v>12928</v>
+        <v>41660</v>
       </c>
       <c r="C47" s="1">
-        <v>7777260</v>
+        <v>10540600</v>
       </c>
       <c r="D47">
         <v>21</v>
@@ -6885,13 +6888,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>673732</v>
+        <v>2486380</v>
       </c>
       <c r="B48" s="1">
-        <v>54357</v>
+        <v>66816</v>
       </c>
       <c r="C48" s="1">
-        <v>26097200</v>
+        <v>18675400</v>
       </c>
       <c r="D48">
         <v>22</v>
@@ -6902,13 +6905,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>1006000</v>
+        <v>1606800</v>
       </c>
       <c r="B49" s="1">
-        <v>59876</v>
+        <v>84610</v>
       </c>
       <c r="C49" s="1">
-        <v>50709400</v>
+        <v>30119300</v>
       </c>
       <c r="D49">
         <v>23</v>
@@ -6919,13 +6922,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1424090</v>
+        <v>4336600</v>
       </c>
       <c r="B50" s="1">
-        <v>36336</v>
+        <v>122667</v>
       </c>
       <c r="C50" s="1">
-        <v>76291900</v>
+        <v>51455400</v>
       </c>
       <c r="D50">
         <v>24</v>
@@ -6936,13 +6939,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>1905310</v>
+        <v>5761340</v>
       </c>
       <c r="B51" s="1">
-        <v>51352</v>
+        <v>163950</v>
       </c>
       <c r="C51" s="1">
-        <v>137391000</v>
+        <v>99136200</v>
       </c>
       <c r="D51">
         <v>25</v>
@@ -6953,13 +6956,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>2699150</v>
+        <v>8044690</v>
       </c>
       <c r="B52" s="1">
-        <v>72816</v>
+        <v>64980</v>
       </c>
       <c r="C52" s="1">
-        <v>250417000</v>
+        <v>159232000</v>
       </c>
       <c r="D52">
         <v>26</v>
@@ -6970,13 +6973,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>92</v>
+        <v>800</v>
       </c>
       <c r="B53" s="1">
-        <v>24</v>
+        <v>1060</v>
       </c>
       <c r="C53" s="1">
-        <v>192</v>
+        <v>1010</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -6987,13 +6990,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>816</v>
+        <v>13710</v>
       </c>
       <c r="B54">
-        <v>264</v>
+        <v>1513</v>
       </c>
       <c r="C54" s="1">
-        <v>336</v>
+        <v>2320</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -7004,13 +7007,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>684</v>
+        <v>14870</v>
       </c>
       <c r="B55" s="1">
-        <v>396</v>
+        <v>2390</v>
       </c>
       <c r="C55">
-        <v>456</v>
+        <v>1885</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -7021,13 +7024,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>24776</v>
+        <v>17220</v>
       </c>
       <c r="B56" s="1">
-        <v>576</v>
+        <v>3300</v>
       </c>
       <c r="C56" s="1">
-        <v>592</v>
+        <v>2780</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -7038,13 +7041,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>1452</v>
+        <v>17610</v>
       </c>
       <c r="B57" s="1">
-        <v>1004</v>
+        <v>3301</v>
       </c>
       <c r="C57" s="1">
-        <v>964</v>
+        <v>3560</v>
       </c>
       <c r="D57">
         <v>5</v>
@@ -7055,13 +7058,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>1836</v>
+        <v>15238</v>
       </c>
       <c r="B58">
-        <v>1572</v>
+        <v>6660</v>
       </c>
       <c r="C58" s="1">
-        <v>1408</v>
+        <v>3652</v>
       </c>
       <c r="D58">
         <v>6</v>
@@ -7072,13 +7075,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>2848</v>
+        <v>45640</v>
       </c>
       <c r="B59" s="1">
-        <v>2236</v>
+        <v>7310</v>
       </c>
       <c r="C59" s="1">
-        <v>2444</v>
+        <v>7850</v>
       </c>
       <c r="D59">
         <v>7</v>
@@ -7089,13 +7092,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>3572</v>
+        <v>41440</v>
       </c>
       <c r="B60" s="1">
-        <v>3628</v>
+        <v>7115</v>
       </c>
       <c r="C60" s="1">
-        <v>14966</v>
+        <v>12900</v>
       </c>
       <c r="D60">
         <v>8</v>
@@ -7106,13 +7109,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>52305</v>
+        <v>47010</v>
       </c>
       <c r="B61" s="1">
-        <v>26829</v>
+        <v>21480</v>
       </c>
       <c r="C61" s="1">
-        <v>26169</v>
+        <v>21350</v>
       </c>
       <c r="D61">
         <v>9</v>
@@ -7123,13 +7126,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>29403</v>
+        <v>32880</v>
       </c>
       <c r="B62" s="1">
-        <v>45425</v>
+        <v>25565</v>
       </c>
       <c r="C62" s="1">
-        <v>44500</v>
+        <v>47690</v>
       </c>
       <c r="D62">
         <v>10</v>
@@ -7140,13 +7143,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>44484</v>
+        <v>67180</v>
       </c>
       <c r="B63" s="1">
-        <v>80883</v>
+        <v>80908</v>
       </c>
       <c r="C63" s="1">
-        <v>84595</v>
+        <v>84840</v>
       </c>
       <c r="D63">
         <v>11</v>
@@ -7157,13 +7160,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>71131</v>
+        <v>88620</v>
       </c>
       <c r="B64" s="1">
-        <v>158994</v>
+        <v>128710</v>
       </c>
       <c r="C64" s="1">
-        <v>167871</v>
+        <v>371329</v>
       </c>
       <c r="D64">
         <v>12</v>
@@ -7174,13 +7177,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>101508</v>
+        <v>145944</v>
       </c>
       <c r="B65" s="1">
-        <v>317724</v>
+        <v>113736</v>
       </c>
       <c r="C65" s="1">
-        <v>330231</v>
+        <v>164249</v>
       </c>
       <c r="D65">
         <v>13</v>
@@ -7191,13 +7194,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>142824</v>
+        <v>79812</v>
       </c>
       <c r="B66" s="1">
-        <v>622512</v>
+        <v>254320</v>
       </c>
       <c r="C66" s="1">
-        <v>647361</v>
+        <v>679613</v>
       </c>
       <c r="D66">
         <v>14</v>
@@ -7208,13 +7211,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>236131</v>
+        <v>461002</v>
       </c>
       <c r="B67" s="1">
-        <v>1226590</v>
+        <v>1208500</v>
       </c>
       <c r="C67" s="1">
-        <v>1288800</v>
+        <v>1168080</v>
       </c>
       <c r="D67">
         <v>15</v>
@@ -7225,13 +7228,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>293518</v>
+        <v>367880</v>
       </c>
       <c r="B68" s="1">
-        <v>2433140</v>
+        <v>1893510</v>
       </c>
       <c r="C68" s="1">
-        <v>2570020</v>
+        <v>2202340</v>
       </c>
       <c r="D68">
         <v>16</v>
@@ -7242,13 +7245,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>418489</v>
+        <v>287345</v>
       </c>
       <c r="B69" s="1">
-        <v>4877550</v>
+        <v>3548520</v>
       </c>
       <c r="C69" s="1">
-        <v>5112610</v>
+        <v>3214680</v>
       </c>
       <c r="D69">
         <v>17</v>
@@ -7259,13 +7262,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>607794</v>
+        <v>528981</v>
       </c>
       <c r="B70" s="1">
-        <v>9721900</v>
+        <v>5143060</v>
       </c>
       <c r="C70" s="1">
-        <v>10049800</v>
+        <v>6590370</v>
       </c>
       <c r="D70">
         <v>18</v>
@@ -7276,13 +7279,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>727373</v>
+        <v>726737</v>
       </c>
       <c r="B71" s="1">
-        <v>17846500</v>
+        <v>11032700</v>
       </c>
       <c r="C71" s="1">
-        <v>13852800</v>
+        <v>12313900</v>
       </c>
       <c r="D71">
         <v>19</v>
@@ -7293,13 +7296,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>1302790</v>
+        <v>1354050</v>
       </c>
       <c r="B72" s="1">
-        <v>24192500</v>
+        <v>18947300</v>
       </c>
       <c r="C72" s="1">
-        <v>9463410</v>
+        <v>23168200</v>
       </c>
       <c r="D72">
         <v>20</v>
@@ -7309,14 +7312,14 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>469364</v>
+      <c r="A73" s="1">
+        <v>1367560</v>
       </c>
       <c r="B73" s="1">
-        <v>27404700</v>
+        <v>31632800</v>
       </c>
       <c r="C73" s="1">
-        <v>40634300</v>
+        <v>33783100</v>
       </c>
       <c r="D73">
         <v>21</v>
@@ -7327,13 +7330,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>1821350</v>
+        <v>2425840</v>
       </c>
       <c r="B74" s="1">
-        <v>57176400</v>
+        <v>50460700</v>
       </c>
       <c r="C74" s="1">
-        <v>48241400</v>
+        <v>69251500</v>
       </c>
       <c r="D74">
         <v>22</v>
@@ -7343,14 +7346,14 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>980792</v>
+      <c r="A75" s="1">
+        <v>3394910</v>
       </c>
       <c r="B75" s="1">
-        <v>76641300</v>
+        <v>97757100</v>
       </c>
       <c r="C75" s="1">
-        <v>85835600</v>
+        <v>117393000</v>
       </c>
       <c r="D75">
         <v>23</v>
@@ -7361,13 +7364,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>1406840</v>
+        <v>4505120</v>
       </c>
       <c r="B76" s="1">
-        <v>143156000</v>
+        <v>162686000</v>
       </c>
       <c r="C76" s="1">
-        <v>169027000</v>
+        <v>190406000</v>
       </c>
       <c r="D76">
         <v>24</v>
@@ -7378,13 +7381,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>1857820</v>
+        <v>6077040</v>
       </c>
       <c r="B77" s="1">
-        <v>286863000</v>
+        <v>333139000</v>
       </c>
       <c r="C77" s="1">
-        <v>302730000</v>
+        <v>384898000</v>
       </c>
       <c r="D77">
         <v>25</v>
@@ -7395,13 +7398,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>2650960</v>
+        <v>7564420</v>
       </c>
       <c r="B78" s="1">
-        <v>559201000</v>
+        <v>648790000</v>
       </c>
       <c r="C78" s="1">
-        <v>571163000</v>
+        <v>803016000</v>
       </c>
       <c r="D78">
         <v>26</v>

</xml_diff>

<commit_message>
Fixed some mistakes; tried to improve write-up.
</commit_message>
<xml_diff>
--- a/chartsnstuff.xlsx
+++ b/chartsnstuff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="27840" windowHeight="16120"/>
+    <workbookView xWindow="11060" yWindow="460" windowWidth="17220" windowHeight="16120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -809,7 +809,7 @@
           <c:idx val="11"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Tim sort Reverse Sorted</c:v>
+            <c:v>Timsort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1625,7 +1625,7 @@
           <c:idx val="10"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Tim sort Presorted</c:v>
+            <c:v>Timsort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2649,11 +2649,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2051636000"/>
-        <c:axId val="-2051387136"/>
+        <c:axId val="-1996952288"/>
+        <c:axId val="-1996946480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2051636000"/>
+        <c:axId val="-1996952288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,11 +2694,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>data</a:t>
+                  <a:t>Data</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> size (4-byte integers)</a:t>
+                  <a:t> Size (4-Byte Integers)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2771,12 +2771,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051387136"/>
+        <c:crossAx val="-1996946480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2051387136"/>
+        <c:axId val="-1996946480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051636000"/>
+        <c:crossAx val="-1996952288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3025,7 +3025,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>(linear scale)</a:t>
+              <a:t>(logarithmic scale)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3693,7 +3693,7 @@
           <c:idx val="11"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Tim sort Reverse Sorted</c:v>
+            <c:v>Timsort Reverse Sorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -4509,7 +4509,7 @@
           <c:idx val="10"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Tim sort Presorted</c:v>
+            <c:v>Timsort Presorted</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -5533,11 +5533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2052040480"/>
-        <c:axId val="-2050008480"/>
+        <c:axId val="-1997300128"/>
+        <c:axId val="-1997294320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2052040480"/>
+        <c:axId val="-1997300128"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5579,11 +5579,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>data</a:t>
+                  <a:t>Data</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> size (4-byte integers)</a:t>
+                  <a:t> Size (4-Byte Integers)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -5656,14 +5656,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050008480"/>
+        <c:crossAx val="-1997294320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="4.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2050008480"/>
+        <c:axId val="-1997294320"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5782,7 +5782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052040480"/>
+        <c:crossAx val="-1997300128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6989,15 +6989,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>233438</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>32578</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>538238</xdr:colOff>
+      <xdr:colOff>346213</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>7604</xdr:rowOff>
+      <xdr:rowOff>131843</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7318,8 +7318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="92" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>